<commit_message>
update data biaya mds
</commit_message>
<xml_diff>
--- a/SPP.xlsx
+++ b/SPP.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19890" windowHeight="8370"/>
+    <workbookView windowWidth="19890" windowHeight="8370" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="4" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110">
   <si>
     <t>Count of SPP</t>
   </si>
@@ -332,6 +332,24 @@
   <si>
     <t>Non Pendidikan</t>
   </si>
+  <si>
+    <t>HAMAM BIN MULYONO</t>
+  </si>
+  <si>
+    <t>AZKA AL ATHAF</t>
+  </si>
+  <si>
+    <t>MUHAMMAD RIZQI ADIK ILHAM</t>
+  </si>
+  <si>
+    <t>NAWAZ</t>
+  </si>
+  <si>
+    <t>FAQIH</t>
+  </si>
+  <si>
+    <t>MUHAMMAD ABDUL MU'THI</t>
+  </si>
 </sst>
 </file>
 
@@ -340,10 +358,10 @@
   <numFmts count="6">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="m/d/yyyy;@"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -362,6 +380,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -369,16 +395,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -391,11 +440,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -408,7 +456,15 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -424,38 +480,23 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -468,24 +509,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -493,14 +519,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -515,25 +533,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -545,97 +599,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -653,13 +617,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -671,13 +635,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -693,12 +717,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -709,13 +727,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -725,6 +747,15 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -759,15 +790,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -786,23 +808,19 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -811,13 +829,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -829,130 +847,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -14502,7 +14520,1021 @@
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" autoFormatId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" createdVersion="5" useAutoFormatting="1" compact="0" indent="0" outline="1" compactData="0" outlineData="1" showDrill="1" multipleFieldFilters="0">
   <location ref="A3:R95" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="10">
-    <pivotField compact="0" showAll="0"/>
+    <pivotField compact="0" showAll="0">
+      <items count="1011">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="36"/>
+        <item x="37"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="40"/>
+        <item x="41"/>
+        <item x="42"/>
+        <item x="43"/>
+        <item x="44"/>
+        <item x="45"/>
+        <item x="46"/>
+        <item x="47"/>
+        <item x="48"/>
+        <item x="49"/>
+        <item x="50"/>
+        <item x="51"/>
+        <item x="52"/>
+        <item x="53"/>
+        <item x="54"/>
+        <item x="55"/>
+        <item x="56"/>
+        <item x="57"/>
+        <item x="58"/>
+        <item x="59"/>
+        <item x="60"/>
+        <item x="61"/>
+        <item x="62"/>
+        <item x="63"/>
+        <item x="64"/>
+        <item x="65"/>
+        <item x="66"/>
+        <item x="67"/>
+        <item x="68"/>
+        <item x="69"/>
+        <item x="70"/>
+        <item x="71"/>
+        <item x="72"/>
+        <item x="73"/>
+        <item x="74"/>
+        <item x="75"/>
+        <item x="76"/>
+        <item x="77"/>
+        <item x="78"/>
+        <item x="79"/>
+        <item x="80"/>
+        <item x="81"/>
+        <item x="82"/>
+        <item x="83"/>
+        <item x="84"/>
+        <item x="85"/>
+        <item x="86"/>
+        <item x="87"/>
+        <item x="88"/>
+        <item x="89"/>
+        <item x="90"/>
+        <item x="91"/>
+        <item x="92"/>
+        <item x="93"/>
+        <item x="94"/>
+        <item x="95"/>
+        <item x="96"/>
+        <item x="97"/>
+        <item x="98"/>
+        <item x="99"/>
+        <item x="100"/>
+        <item x="101"/>
+        <item x="102"/>
+        <item x="103"/>
+        <item x="104"/>
+        <item x="105"/>
+        <item x="106"/>
+        <item x="107"/>
+        <item x="108"/>
+        <item x="109"/>
+        <item x="110"/>
+        <item x="111"/>
+        <item x="112"/>
+        <item x="113"/>
+        <item x="114"/>
+        <item x="115"/>
+        <item x="116"/>
+        <item x="117"/>
+        <item x="118"/>
+        <item x="119"/>
+        <item x="120"/>
+        <item x="121"/>
+        <item x="122"/>
+        <item x="123"/>
+        <item x="124"/>
+        <item x="125"/>
+        <item x="126"/>
+        <item x="127"/>
+        <item x="128"/>
+        <item x="129"/>
+        <item x="130"/>
+        <item x="131"/>
+        <item x="132"/>
+        <item x="133"/>
+        <item x="134"/>
+        <item x="135"/>
+        <item x="136"/>
+        <item x="137"/>
+        <item x="138"/>
+        <item x="139"/>
+        <item x="140"/>
+        <item x="141"/>
+        <item x="142"/>
+        <item x="143"/>
+        <item x="144"/>
+        <item x="145"/>
+        <item x="146"/>
+        <item x="147"/>
+        <item x="148"/>
+        <item x="149"/>
+        <item x="150"/>
+        <item x="151"/>
+        <item x="152"/>
+        <item x="153"/>
+        <item x="154"/>
+        <item x="155"/>
+        <item x="156"/>
+        <item x="157"/>
+        <item x="158"/>
+        <item x="159"/>
+        <item x="160"/>
+        <item x="161"/>
+        <item x="162"/>
+        <item x="163"/>
+        <item x="164"/>
+        <item x="165"/>
+        <item x="166"/>
+        <item x="167"/>
+        <item x="168"/>
+        <item x="169"/>
+        <item x="170"/>
+        <item x="171"/>
+        <item x="172"/>
+        <item x="173"/>
+        <item x="174"/>
+        <item x="175"/>
+        <item x="176"/>
+        <item x="177"/>
+        <item x="178"/>
+        <item x="179"/>
+        <item x="180"/>
+        <item x="181"/>
+        <item x="182"/>
+        <item x="183"/>
+        <item x="184"/>
+        <item x="185"/>
+        <item x="186"/>
+        <item x="187"/>
+        <item x="188"/>
+        <item x="189"/>
+        <item x="190"/>
+        <item x="191"/>
+        <item x="192"/>
+        <item x="193"/>
+        <item x="194"/>
+        <item x="195"/>
+        <item x="196"/>
+        <item x="197"/>
+        <item x="198"/>
+        <item x="199"/>
+        <item x="200"/>
+        <item x="201"/>
+        <item x="202"/>
+        <item x="203"/>
+        <item x="204"/>
+        <item x="205"/>
+        <item x="206"/>
+        <item x="207"/>
+        <item x="208"/>
+        <item x="209"/>
+        <item x="210"/>
+        <item x="211"/>
+        <item x="212"/>
+        <item x="213"/>
+        <item x="214"/>
+        <item x="215"/>
+        <item x="216"/>
+        <item x="217"/>
+        <item x="218"/>
+        <item x="219"/>
+        <item x="220"/>
+        <item x="221"/>
+        <item x="222"/>
+        <item x="223"/>
+        <item x="224"/>
+        <item x="225"/>
+        <item x="226"/>
+        <item x="227"/>
+        <item x="228"/>
+        <item x="229"/>
+        <item x="230"/>
+        <item x="231"/>
+        <item x="232"/>
+        <item x="233"/>
+        <item x="234"/>
+        <item x="235"/>
+        <item x="236"/>
+        <item x="237"/>
+        <item x="238"/>
+        <item x="239"/>
+        <item x="240"/>
+        <item x="241"/>
+        <item x="242"/>
+        <item x="243"/>
+        <item x="244"/>
+        <item x="245"/>
+        <item x="246"/>
+        <item x="247"/>
+        <item x="248"/>
+        <item x="249"/>
+        <item x="250"/>
+        <item x="251"/>
+        <item x="252"/>
+        <item x="253"/>
+        <item x="254"/>
+        <item x="255"/>
+        <item x="256"/>
+        <item x="257"/>
+        <item x="258"/>
+        <item x="259"/>
+        <item x="260"/>
+        <item x="261"/>
+        <item x="262"/>
+        <item x="263"/>
+        <item x="264"/>
+        <item x="265"/>
+        <item x="266"/>
+        <item x="267"/>
+        <item x="268"/>
+        <item x="269"/>
+        <item x="270"/>
+        <item x="271"/>
+        <item x="272"/>
+        <item x="273"/>
+        <item x="274"/>
+        <item x="275"/>
+        <item x="276"/>
+        <item x="277"/>
+        <item x="278"/>
+        <item x="279"/>
+        <item x="280"/>
+        <item x="281"/>
+        <item x="282"/>
+        <item x="283"/>
+        <item x="284"/>
+        <item x="285"/>
+        <item x="286"/>
+        <item x="287"/>
+        <item x="288"/>
+        <item x="289"/>
+        <item x="290"/>
+        <item x="291"/>
+        <item x="292"/>
+        <item x="293"/>
+        <item x="294"/>
+        <item x="295"/>
+        <item x="296"/>
+        <item x="297"/>
+        <item x="298"/>
+        <item x="299"/>
+        <item x="300"/>
+        <item x="301"/>
+        <item x="302"/>
+        <item x="303"/>
+        <item x="304"/>
+        <item x="305"/>
+        <item x="306"/>
+        <item x="307"/>
+        <item x="308"/>
+        <item x="309"/>
+        <item x="310"/>
+        <item x="311"/>
+        <item x="312"/>
+        <item x="313"/>
+        <item x="314"/>
+        <item x="315"/>
+        <item x="316"/>
+        <item x="317"/>
+        <item x="318"/>
+        <item x="319"/>
+        <item x="320"/>
+        <item x="321"/>
+        <item x="322"/>
+        <item x="323"/>
+        <item x="324"/>
+        <item x="325"/>
+        <item x="326"/>
+        <item x="327"/>
+        <item x="328"/>
+        <item x="329"/>
+        <item x="330"/>
+        <item x="331"/>
+        <item x="332"/>
+        <item x="333"/>
+        <item x="334"/>
+        <item x="335"/>
+        <item x="336"/>
+        <item x="337"/>
+        <item x="338"/>
+        <item x="339"/>
+        <item x="340"/>
+        <item x="341"/>
+        <item x="342"/>
+        <item x="343"/>
+        <item x="344"/>
+        <item x="345"/>
+        <item x="346"/>
+        <item x="347"/>
+        <item x="348"/>
+        <item x="349"/>
+        <item x="350"/>
+        <item x="351"/>
+        <item x="352"/>
+        <item x="353"/>
+        <item x="354"/>
+        <item x="355"/>
+        <item x="356"/>
+        <item x="357"/>
+        <item x="358"/>
+        <item x="359"/>
+        <item x="360"/>
+        <item x="361"/>
+        <item x="362"/>
+        <item x="363"/>
+        <item x="364"/>
+        <item x="365"/>
+        <item x="366"/>
+        <item x="367"/>
+        <item x="368"/>
+        <item x="369"/>
+        <item x="370"/>
+        <item x="371"/>
+        <item x="372"/>
+        <item x="373"/>
+        <item x="374"/>
+        <item x="375"/>
+        <item x="376"/>
+        <item x="377"/>
+        <item x="378"/>
+        <item x="379"/>
+        <item x="380"/>
+        <item x="381"/>
+        <item x="382"/>
+        <item x="383"/>
+        <item x="384"/>
+        <item x="385"/>
+        <item x="386"/>
+        <item x="387"/>
+        <item x="388"/>
+        <item x="389"/>
+        <item x="390"/>
+        <item x="391"/>
+        <item x="392"/>
+        <item x="393"/>
+        <item x="394"/>
+        <item x="395"/>
+        <item x="396"/>
+        <item x="397"/>
+        <item x="398"/>
+        <item x="399"/>
+        <item x="400"/>
+        <item x="401"/>
+        <item x="402"/>
+        <item x="403"/>
+        <item x="404"/>
+        <item x="405"/>
+        <item x="406"/>
+        <item x="407"/>
+        <item x="408"/>
+        <item x="409"/>
+        <item x="410"/>
+        <item x="411"/>
+        <item x="412"/>
+        <item x="413"/>
+        <item x="414"/>
+        <item x="415"/>
+        <item x="416"/>
+        <item x="417"/>
+        <item x="418"/>
+        <item x="419"/>
+        <item x="420"/>
+        <item x="421"/>
+        <item x="422"/>
+        <item x="423"/>
+        <item x="424"/>
+        <item x="425"/>
+        <item x="426"/>
+        <item x="427"/>
+        <item x="428"/>
+        <item x="429"/>
+        <item x="430"/>
+        <item x="431"/>
+        <item x="432"/>
+        <item x="433"/>
+        <item x="434"/>
+        <item x="435"/>
+        <item x="436"/>
+        <item x="437"/>
+        <item x="438"/>
+        <item x="439"/>
+        <item x="440"/>
+        <item x="441"/>
+        <item x="442"/>
+        <item x="443"/>
+        <item x="444"/>
+        <item x="445"/>
+        <item x="446"/>
+        <item x="447"/>
+        <item x="448"/>
+        <item x="449"/>
+        <item x="450"/>
+        <item x="451"/>
+        <item x="452"/>
+        <item x="453"/>
+        <item x="454"/>
+        <item x="455"/>
+        <item x="456"/>
+        <item x="457"/>
+        <item x="458"/>
+        <item x="459"/>
+        <item x="460"/>
+        <item x="461"/>
+        <item x="462"/>
+        <item x="463"/>
+        <item x="464"/>
+        <item x="465"/>
+        <item x="466"/>
+        <item x="467"/>
+        <item x="468"/>
+        <item x="469"/>
+        <item x="470"/>
+        <item x="471"/>
+        <item x="472"/>
+        <item x="473"/>
+        <item x="474"/>
+        <item x="475"/>
+        <item x="476"/>
+        <item x="477"/>
+        <item x="478"/>
+        <item x="479"/>
+        <item x="480"/>
+        <item x="481"/>
+        <item x="482"/>
+        <item x="483"/>
+        <item x="484"/>
+        <item x="485"/>
+        <item x="486"/>
+        <item x="487"/>
+        <item x="488"/>
+        <item x="489"/>
+        <item x="490"/>
+        <item x="491"/>
+        <item x="492"/>
+        <item x="493"/>
+        <item x="494"/>
+        <item x="495"/>
+        <item x="496"/>
+        <item x="497"/>
+        <item x="498"/>
+        <item x="499"/>
+        <item x="500"/>
+        <item x="501"/>
+        <item x="502"/>
+        <item x="503"/>
+        <item x="504"/>
+        <item x="505"/>
+        <item x="506"/>
+        <item x="507"/>
+        <item x="508"/>
+        <item x="509"/>
+        <item x="510"/>
+        <item x="511"/>
+        <item x="512"/>
+        <item x="513"/>
+        <item x="514"/>
+        <item x="515"/>
+        <item x="516"/>
+        <item x="517"/>
+        <item x="518"/>
+        <item x="519"/>
+        <item x="520"/>
+        <item x="521"/>
+        <item x="522"/>
+        <item x="523"/>
+        <item x="524"/>
+        <item x="525"/>
+        <item x="526"/>
+        <item x="527"/>
+        <item x="528"/>
+        <item x="529"/>
+        <item x="530"/>
+        <item x="531"/>
+        <item x="532"/>
+        <item x="533"/>
+        <item x="534"/>
+        <item x="535"/>
+        <item x="536"/>
+        <item x="537"/>
+        <item x="538"/>
+        <item x="539"/>
+        <item x="540"/>
+        <item x="541"/>
+        <item x="542"/>
+        <item x="543"/>
+        <item x="544"/>
+        <item x="545"/>
+        <item x="546"/>
+        <item x="547"/>
+        <item x="548"/>
+        <item x="549"/>
+        <item x="550"/>
+        <item x="551"/>
+        <item x="552"/>
+        <item x="553"/>
+        <item x="554"/>
+        <item x="555"/>
+        <item x="556"/>
+        <item x="557"/>
+        <item x="558"/>
+        <item x="559"/>
+        <item x="560"/>
+        <item x="561"/>
+        <item x="562"/>
+        <item x="563"/>
+        <item x="564"/>
+        <item x="565"/>
+        <item x="566"/>
+        <item x="567"/>
+        <item x="568"/>
+        <item x="569"/>
+        <item x="570"/>
+        <item x="571"/>
+        <item x="572"/>
+        <item x="573"/>
+        <item x="574"/>
+        <item x="575"/>
+        <item x="576"/>
+        <item x="577"/>
+        <item x="578"/>
+        <item x="579"/>
+        <item x="580"/>
+        <item x="581"/>
+        <item x="582"/>
+        <item x="583"/>
+        <item x="584"/>
+        <item x="585"/>
+        <item x="586"/>
+        <item x="587"/>
+        <item x="588"/>
+        <item x="589"/>
+        <item x="590"/>
+        <item x="591"/>
+        <item x="592"/>
+        <item x="593"/>
+        <item x="594"/>
+        <item x="595"/>
+        <item x="596"/>
+        <item x="597"/>
+        <item x="598"/>
+        <item x="599"/>
+        <item x="600"/>
+        <item x="601"/>
+        <item x="602"/>
+        <item x="603"/>
+        <item x="604"/>
+        <item x="605"/>
+        <item x="606"/>
+        <item x="607"/>
+        <item x="608"/>
+        <item x="609"/>
+        <item x="610"/>
+        <item x="611"/>
+        <item x="612"/>
+        <item x="613"/>
+        <item x="614"/>
+        <item x="615"/>
+        <item x="616"/>
+        <item x="617"/>
+        <item x="618"/>
+        <item x="619"/>
+        <item x="620"/>
+        <item x="621"/>
+        <item x="622"/>
+        <item x="623"/>
+        <item x="624"/>
+        <item x="625"/>
+        <item x="626"/>
+        <item x="627"/>
+        <item x="628"/>
+        <item x="629"/>
+        <item x="630"/>
+        <item x="631"/>
+        <item x="632"/>
+        <item x="633"/>
+        <item x="634"/>
+        <item x="635"/>
+        <item x="636"/>
+        <item x="637"/>
+        <item x="638"/>
+        <item x="639"/>
+        <item x="640"/>
+        <item x="641"/>
+        <item x="642"/>
+        <item x="643"/>
+        <item x="644"/>
+        <item x="645"/>
+        <item x="646"/>
+        <item x="647"/>
+        <item x="648"/>
+        <item x="649"/>
+        <item x="650"/>
+        <item x="651"/>
+        <item x="652"/>
+        <item x="653"/>
+        <item x="654"/>
+        <item x="655"/>
+        <item x="656"/>
+        <item x="657"/>
+        <item x="658"/>
+        <item x="659"/>
+        <item x="660"/>
+        <item x="661"/>
+        <item x="662"/>
+        <item x="663"/>
+        <item x="664"/>
+        <item x="665"/>
+        <item x="666"/>
+        <item x="667"/>
+        <item x="668"/>
+        <item x="669"/>
+        <item x="670"/>
+        <item x="671"/>
+        <item x="672"/>
+        <item x="673"/>
+        <item x="674"/>
+        <item x="675"/>
+        <item x="676"/>
+        <item x="677"/>
+        <item x="678"/>
+        <item x="679"/>
+        <item x="680"/>
+        <item x="681"/>
+        <item x="682"/>
+        <item x="683"/>
+        <item x="684"/>
+        <item x="685"/>
+        <item x="686"/>
+        <item x="687"/>
+        <item x="688"/>
+        <item x="689"/>
+        <item x="690"/>
+        <item x="691"/>
+        <item x="692"/>
+        <item x="693"/>
+        <item x="694"/>
+        <item x="695"/>
+        <item x="696"/>
+        <item x="697"/>
+        <item x="698"/>
+        <item x="699"/>
+        <item x="700"/>
+        <item x="701"/>
+        <item x="702"/>
+        <item x="703"/>
+        <item x="704"/>
+        <item x="705"/>
+        <item x="706"/>
+        <item x="707"/>
+        <item x="708"/>
+        <item x="709"/>
+        <item x="710"/>
+        <item x="711"/>
+        <item x="712"/>
+        <item x="713"/>
+        <item x="714"/>
+        <item x="715"/>
+        <item x="716"/>
+        <item x="717"/>
+        <item x="718"/>
+        <item x="719"/>
+        <item x="720"/>
+        <item x="721"/>
+        <item x="722"/>
+        <item x="723"/>
+        <item x="724"/>
+        <item x="725"/>
+        <item x="726"/>
+        <item x="727"/>
+        <item x="728"/>
+        <item x="729"/>
+        <item x="730"/>
+        <item x="731"/>
+        <item x="732"/>
+        <item x="733"/>
+        <item x="734"/>
+        <item x="735"/>
+        <item x="736"/>
+        <item x="737"/>
+        <item x="738"/>
+        <item x="739"/>
+        <item x="740"/>
+        <item x="741"/>
+        <item x="742"/>
+        <item x="743"/>
+        <item x="744"/>
+        <item x="745"/>
+        <item x="746"/>
+        <item x="747"/>
+        <item x="748"/>
+        <item x="749"/>
+        <item x="750"/>
+        <item x="751"/>
+        <item x="752"/>
+        <item x="753"/>
+        <item x="754"/>
+        <item x="755"/>
+        <item x="756"/>
+        <item x="757"/>
+        <item x="758"/>
+        <item x="759"/>
+        <item x="760"/>
+        <item x="761"/>
+        <item x="762"/>
+        <item x="763"/>
+        <item x="764"/>
+        <item x="765"/>
+        <item x="766"/>
+        <item x="767"/>
+        <item x="768"/>
+        <item x="769"/>
+        <item x="770"/>
+        <item x="771"/>
+        <item x="772"/>
+        <item x="773"/>
+        <item x="774"/>
+        <item x="775"/>
+        <item x="776"/>
+        <item x="777"/>
+        <item x="778"/>
+        <item x="779"/>
+        <item x="780"/>
+        <item x="781"/>
+        <item x="782"/>
+        <item x="783"/>
+        <item x="784"/>
+        <item x="785"/>
+        <item x="786"/>
+        <item x="787"/>
+        <item x="788"/>
+        <item x="789"/>
+        <item x="790"/>
+        <item x="791"/>
+        <item x="792"/>
+        <item x="793"/>
+        <item x="794"/>
+        <item x="795"/>
+        <item x="796"/>
+        <item x="797"/>
+        <item x="798"/>
+        <item x="799"/>
+        <item x="800"/>
+        <item x="801"/>
+        <item x="802"/>
+        <item x="803"/>
+        <item x="804"/>
+        <item x="805"/>
+        <item x="806"/>
+        <item x="807"/>
+        <item x="808"/>
+        <item x="809"/>
+        <item x="810"/>
+        <item x="811"/>
+        <item x="812"/>
+        <item x="813"/>
+        <item x="814"/>
+        <item x="815"/>
+        <item x="816"/>
+        <item x="817"/>
+        <item x="818"/>
+        <item x="819"/>
+        <item x="820"/>
+        <item x="821"/>
+        <item x="822"/>
+        <item x="823"/>
+        <item x="824"/>
+        <item x="825"/>
+        <item x="826"/>
+        <item x="827"/>
+        <item x="828"/>
+        <item x="829"/>
+        <item x="830"/>
+        <item x="831"/>
+        <item x="832"/>
+        <item x="833"/>
+        <item x="834"/>
+        <item x="835"/>
+        <item x="836"/>
+        <item x="837"/>
+        <item x="838"/>
+        <item x="839"/>
+        <item x="840"/>
+        <item x="841"/>
+        <item x="842"/>
+        <item x="843"/>
+        <item x="844"/>
+        <item x="845"/>
+        <item x="846"/>
+        <item x="847"/>
+        <item x="848"/>
+        <item x="849"/>
+        <item x="850"/>
+        <item x="851"/>
+        <item x="852"/>
+        <item x="853"/>
+        <item x="854"/>
+        <item x="855"/>
+        <item x="856"/>
+        <item x="857"/>
+        <item x="858"/>
+        <item x="859"/>
+        <item x="860"/>
+        <item x="861"/>
+        <item x="862"/>
+        <item x="863"/>
+        <item x="864"/>
+        <item x="865"/>
+        <item x="866"/>
+        <item x="867"/>
+        <item x="868"/>
+        <item x="869"/>
+        <item x="870"/>
+        <item x="871"/>
+        <item x="872"/>
+        <item x="873"/>
+        <item x="874"/>
+        <item x="875"/>
+        <item x="876"/>
+        <item x="877"/>
+        <item x="878"/>
+        <item x="879"/>
+        <item x="880"/>
+        <item x="881"/>
+        <item x="882"/>
+        <item x="883"/>
+        <item x="884"/>
+        <item x="885"/>
+        <item x="886"/>
+        <item x="887"/>
+        <item x="888"/>
+        <item x="889"/>
+        <item x="890"/>
+        <item x="891"/>
+        <item x="892"/>
+        <item x="893"/>
+        <item x="894"/>
+        <item x="895"/>
+        <item x="896"/>
+        <item x="897"/>
+        <item x="898"/>
+        <item x="899"/>
+        <item x="900"/>
+        <item x="901"/>
+        <item x="902"/>
+        <item x="903"/>
+        <item x="904"/>
+        <item x="905"/>
+        <item x="906"/>
+        <item x="907"/>
+        <item x="908"/>
+        <item x="909"/>
+        <item x="910"/>
+        <item x="911"/>
+        <item x="912"/>
+        <item x="913"/>
+        <item x="914"/>
+        <item x="915"/>
+        <item x="916"/>
+        <item x="917"/>
+        <item x="918"/>
+        <item x="919"/>
+        <item x="920"/>
+        <item x="921"/>
+        <item x="922"/>
+        <item x="923"/>
+        <item x="924"/>
+        <item x="925"/>
+        <item x="926"/>
+        <item x="927"/>
+        <item x="928"/>
+        <item x="929"/>
+        <item x="930"/>
+        <item x="931"/>
+        <item x="932"/>
+        <item x="933"/>
+        <item x="934"/>
+        <item x="935"/>
+        <item x="936"/>
+        <item x="937"/>
+        <item x="938"/>
+        <item x="939"/>
+        <item x="940"/>
+        <item x="941"/>
+        <item x="942"/>
+        <item x="943"/>
+        <item x="944"/>
+        <item x="945"/>
+        <item x="946"/>
+        <item x="947"/>
+        <item x="948"/>
+        <item x="949"/>
+        <item x="950"/>
+        <item x="951"/>
+        <item x="952"/>
+        <item x="953"/>
+        <item x="954"/>
+        <item x="955"/>
+        <item x="956"/>
+        <item x="957"/>
+        <item x="958"/>
+        <item x="959"/>
+        <item x="960"/>
+        <item x="961"/>
+        <item x="962"/>
+        <item x="963"/>
+        <item x="964"/>
+        <item x="965"/>
+        <item x="966"/>
+        <item x="967"/>
+        <item x="968"/>
+        <item x="969"/>
+        <item x="970"/>
+        <item x="971"/>
+        <item x="972"/>
+        <item x="973"/>
+        <item x="974"/>
+        <item x="975"/>
+        <item x="976"/>
+        <item x="977"/>
+        <item x="978"/>
+        <item x="979"/>
+        <item x="980"/>
+        <item x="981"/>
+        <item x="982"/>
+        <item x="983"/>
+        <item x="984"/>
+        <item x="985"/>
+        <item x="986"/>
+        <item x="987"/>
+        <item x="988"/>
+        <item x="989"/>
+        <item x="990"/>
+        <item x="991"/>
+        <item x="992"/>
+        <item x="993"/>
+        <item x="994"/>
+        <item x="995"/>
+        <item x="996"/>
+        <item x="997"/>
+        <item x="998"/>
+        <item x="999"/>
+        <item x="1000"/>
+        <item x="1001"/>
+        <item x="1002"/>
+        <item x="1003"/>
+        <item x="1004"/>
+        <item x="1005"/>
+        <item x="1006"/>
+        <item x="1007"/>
+        <item x="1008"/>
+        <item x="1009"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
     <pivotField axis="axisRow" compact="0" showAll="0">
       <items count="90">
         <item x="55"/>
@@ -14601,7 +15633,24 @@
     <pivotField compact="0" showAll="0"/>
     <pivotField compact="0" showAll="0"/>
     <pivotField compact="0" showAll="0"/>
-    <pivotField dataField="1" compact="0" showAll="0"/>
+    <pivotField dataField="1" compact="0" showAll="0">
+      <items count="14">
+        <item x="11"/>
+        <item x="10"/>
+        <item x="8"/>
+        <item x="5"/>
+        <item x="3"/>
+        <item x="9"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="4"/>
+        <item x="7"/>
+        <item x="1"/>
+        <item x="6"/>
+        <item x="12"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
     <pivotField compact="0" numFmtId="176" showAll="0"/>
     <pivotField axis="axisCol" compact="0" showAll="0">
       <items count="4">
@@ -15233,7 +16282,7 @@
   <sheetPr/>
   <dimension ref="A3:R95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I16" workbookViewId="0">
+    <sheetView topLeftCell="I16" workbookViewId="0">
       <selection activeCell="X31" sqref="X31"/>
     </sheetView>
   </sheetViews>
@@ -15270,12 +16319,6 @@
       <c r="D4">
         <v>2017</v>
       </c>
-      <c r="E4"/>
-      <c r="F4"/>
-      <c r="G4"/>
-      <c r="H4"/>
-      <c r="I4"/>
-      <c r="J4"/>
       <c r="M4" t="s">
         <v>4</v>
       </c>
@@ -15296,7 +16339,6 @@
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5"/>
       <c r="D5">
         <v>1</v>
       </c>
@@ -15324,7 +16366,6 @@
       <c r="L5">
         <v>12</v>
       </c>
-      <c r="M5"/>
       <c r="N5">
         <v>1</v>
       </c>
@@ -15339,8 +16380,6 @@
       <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6"/>
-      <c r="C6"/>
       <c r="H6">
         <v>2</v>
       </c>
@@ -15364,8 +16403,6 @@
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7"/>
-      <c r="C7"/>
       <c r="G7">
         <v>1</v>
       </c>
@@ -15395,8 +16432,6 @@
       <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B8"/>
-      <c r="C8"/>
       <c r="K8">
         <v>3</v>
       </c>
@@ -15411,8 +16446,6 @@
       <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B9"/>
-      <c r="C9"/>
       <c r="H9">
         <v>1</v>
       </c>
@@ -15439,8 +16472,6 @@
       <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="B10"/>
-      <c r="C10"/>
       <c r="H10">
         <v>2</v>
       </c>
@@ -15467,8 +16498,6 @@
       <c r="A11" t="s">
         <v>13</v>
       </c>
-      <c r="B11"/>
-      <c r="C11"/>
       <c r="H11">
         <v>2</v>
       </c>
@@ -15501,8 +16530,6 @@
       <c r="A12" t="s">
         <v>14</v>
       </c>
-      <c r="B12"/>
-      <c r="C12"/>
       <c r="G12">
         <v>1</v>
       </c>
@@ -15538,8 +16565,6 @@
       <c r="A13" t="s">
         <v>15</v>
       </c>
-      <c r="B13"/>
-      <c r="C13"/>
       <c r="G13">
         <v>1</v>
       </c>
@@ -15569,8 +16594,6 @@
       <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="B14"/>
-      <c r="C14"/>
       <c r="G14">
         <v>1</v>
       </c>
@@ -15597,8 +16620,6 @@
       <c r="A15" t="s">
         <v>17</v>
       </c>
-      <c r="B15"/>
-      <c r="C15"/>
       <c r="G15">
         <v>1</v>
       </c>
@@ -15625,8 +16646,6 @@
       <c r="A16" t="s">
         <v>18</v>
       </c>
-      <c r="B16"/>
-      <c r="C16"/>
       <c r="G16">
         <v>1</v>
       </c>
@@ -15662,8 +16681,6 @@
       <c r="A17" t="s">
         <v>19</v>
       </c>
-      <c r="B17"/>
-      <c r="C17"/>
       <c r="G17">
         <v>1</v>
       </c>
@@ -15699,8 +16716,6 @@
       <c r="A18" t="s">
         <v>20</v>
       </c>
-      <c r="B18"/>
-      <c r="C18"/>
       <c r="G18">
         <v>1</v>
       </c>
@@ -15736,8 +16751,6 @@
       <c r="A19" t="s">
         <v>21</v>
       </c>
-      <c r="B19"/>
-      <c r="C19"/>
       <c r="G19">
         <v>3</v>
       </c>
@@ -15761,8 +16774,6 @@
       <c r="A20" t="s">
         <v>22</v>
       </c>
-      <c r="B20"/>
-      <c r="C20"/>
       <c r="N20">
         <v>6</v>
       </c>
@@ -17812,16 +18823,16 @@
   <sheetPr/>
   <dimension ref="A1:J1011"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A988" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A555" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A1011" sqref="A1:J1011"/>
+      <selection pane="bottomLeft" activeCell="E572" sqref="E572"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.71428571428571" customWidth="1"/>
-    <col min="2" max="2" width="27.1428571428571" customWidth="1"/>
+    <col min="2" max="2" width="33.4285714285714" customWidth="1"/>
     <col min="5" max="5" width="11.4285714285714" style="1"/>
     <col min="6" max="6" width="12.4285714285714" style="2" customWidth="1"/>
     <col min="7" max="7" width="12.8571428571429" style="3"/>
@@ -35797,20 +36808,35 @@
         <f t="shared" si="42"/>
         <v>539</v>
       </c>
+      <c r="B540" t="s">
+        <v>104</v>
+      </c>
       <c r="C540">
         <v>1</v>
+      </c>
+      <c r="D540">
+        <v>9</v>
+      </c>
+      <c r="E540" s="1">
+        <v>42987</v>
+      </c>
+      <c r="F540" s="2">
+        <v>2377</v>
+      </c>
+      <c r="G540" s="3">
+        <v>150000</v>
       </c>
       <c r="H540" s="3">
         <f t="shared" si="41"/>
-        <v>-150000</v>
+        <v>0</v>
       </c>
       <c r="I540" s="4">
         <f t="shared" si="43"/>
-        <v>1900</v>
+        <v>2017</v>
       </c>
       <c r="J540">
         <f t="shared" si="44"/>
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="541" spans="1:10">
@@ -35818,20 +36844,35 @@
         <f t="shared" si="42"/>
         <v>540</v>
       </c>
+      <c r="B541" t="s">
+        <v>104</v>
+      </c>
       <c r="C541">
         <v>1</v>
+      </c>
+      <c r="D541">
+        <v>10</v>
+      </c>
+      <c r="E541" s="1">
+        <v>43092</v>
+      </c>
+      <c r="F541" s="2">
+        <v>1684</v>
+      </c>
+      <c r="G541" s="3">
+        <v>150000</v>
       </c>
       <c r="H541" s="3">
         <f t="shared" si="41"/>
-        <v>-150000</v>
+        <v>0</v>
       </c>
       <c r="I541" s="4">
         <f t="shared" si="43"/>
-        <v>1900</v>
+        <v>2017</v>
       </c>
       <c r="J541">
         <f t="shared" si="44"/>
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="542" spans="1:10">
@@ -35839,20 +36880,35 @@
         <f t="shared" si="42"/>
         <v>541</v>
       </c>
+      <c r="B542" t="s">
+        <v>104</v>
+      </c>
       <c r="C542">
         <v>1</v>
+      </c>
+      <c r="D542">
+        <v>11</v>
+      </c>
+      <c r="E542" s="1">
+        <v>43092</v>
+      </c>
+      <c r="F542" s="2">
+        <v>1684</v>
+      </c>
+      <c r="G542" s="3">
+        <v>150000</v>
       </c>
       <c r="H542" s="3">
         <f t="shared" si="41"/>
-        <v>-150000</v>
+        <v>0</v>
       </c>
       <c r="I542" s="4">
         <f t="shared" si="43"/>
-        <v>1900</v>
+        <v>2017</v>
       </c>
       <c r="J542">
         <f t="shared" si="44"/>
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="543" spans="1:10">
@@ -35860,20 +36916,35 @@
         <f t="shared" si="42"/>
         <v>542</v>
       </c>
+      <c r="B543" t="s">
+        <v>104</v>
+      </c>
       <c r="C543">
         <v>1</v>
+      </c>
+      <c r="D543">
+        <v>12</v>
+      </c>
+      <c r="E543" s="1">
+        <v>43092</v>
+      </c>
+      <c r="F543" s="2">
+        <v>1684</v>
+      </c>
+      <c r="G543" s="3">
+        <v>150000</v>
       </c>
       <c r="H543" s="3">
         <f t="shared" si="41"/>
-        <v>-150000</v>
+        <v>0</v>
       </c>
       <c r="I543" s="4">
         <f t="shared" si="43"/>
-        <v>1900</v>
+        <v>2017</v>
       </c>
       <c r="J543">
         <f t="shared" si="44"/>
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="544" spans="1:10">
@@ -35881,20 +36952,35 @@
         <f t="shared" si="42"/>
         <v>543</v>
       </c>
+      <c r="B544" t="s">
+        <v>105</v>
+      </c>
       <c r="C544">
         <v>1</v>
+      </c>
+      <c r="D544">
+        <v>9</v>
+      </c>
+      <c r="E544" s="1">
+        <v>42987</v>
+      </c>
+      <c r="F544" s="2">
+        <v>2376</v>
+      </c>
+      <c r="G544" s="3">
+        <v>150000</v>
       </c>
       <c r="H544" s="3">
         <f t="shared" si="41"/>
-        <v>-150000</v>
+        <v>0</v>
       </c>
       <c r="I544" s="4">
         <f t="shared" si="43"/>
-        <v>1900</v>
+        <v>2017</v>
       </c>
       <c r="J544">
         <f t="shared" si="44"/>
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="545" spans="1:10">
@@ -35902,20 +36988,35 @@
         <f t="shared" si="42"/>
         <v>544</v>
       </c>
+      <c r="B545" t="s">
+        <v>105</v>
+      </c>
       <c r="C545">
         <v>1</v>
+      </c>
+      <c r="D545">
+        <v>10</v>
+      </c>
+      <c r="E545" s="1">
+        <v>43022</v>
+      </c>
+      <c r="F545" s="2">
+        <v>2546</v>
+      </c>
+      <c r="G545" s="3">
+        <v>150000</v>
       </c>
       <c r="H545" s="3">
         <f t="shared" si="41"/>
-        <v>-150000</v>
+        <v>0</v>
       </c>
       <c r="I545" s="4">
         <f t="shared" si="43"/>
-        <v>1900</v>
+        <v>2017</v>
       </c>
       <c r="J545">
         <f t="shared" si="44"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="546" spans="1:10">
@@ -35923,20 +37024,35 @@
         <f t="shared" si="42"/>
         <v>545</v>
       </c>
+      <c r="B546" t="s">
+        <v>105</v>
+      </c>
       <c r="C546">
         <v>1</v>
+      </c>
+      <c r="D546">
+        <v>11</v>
+      </c>
+      <c r="E546" s="1">
+        <v>43057</v>
+      </c>
+      <c r="F546" s="2">
+        <v>2586</v>
+      </c>
+      <c r="G546" s="3">
+        <v>150000</v>
       </c>
       <c r="H546" s="3">
         <f t="shared" si="41"/>
-        <v>-150000</v>
+        <v>0</v>
       </c>
       <c r="I546" s="4">
         <f t="shared" si="43"/>
-        <v>1900</v>
+        <v>2017</v>
       </c>
       <c r="J546">
         <f t="shared" si="44"/>
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="547" spans="1:10">
@@ -35944,20 +37060,35 @@
         <f t="shared" si="42"/>
         <v>546</v>
       </c>
+      <c r="B547" t="s">
+        <v>105</v>
+      </c>
       <c r="C547">
         <v>1</v>
+      </c>
+      <c r="D547">
+        <v>12</v>
+      </c>
+      <c r="E547" s="1">
+        <v>43085</v>
+      </c>
+      <c r="F547" s="2">
+        <v>2657</v>
+      </c>
+      <c r="G547" s="3">
+        <v>150000</v>
       </c>
       <c r="H547" s="3">
         <f t="shared" si="41"/>
-        <v>-150000</v>
+        <v>0</v>
       </c>
       <c r="I547" s="4">
         <f t="shared" si="43"/>
-        <v>1900</v>
+        <v>2017</v>
       </c>
       <c r="J547">
         <f t="shared" si="44"/>
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="548" spans="1:10">
@@ -35965,20 +37096,35 @@
         <f t="shared" si="42"/>
         <v>547</v>
       </c>
+      <c r="B548" t="s">
+        <v>106</v>
+      </c>
       <c r="C548">
         <v>1</v>
+      </c>
+      <c r="D548">
+        <v>9</v>
+      </c>
+      <c r="E548" s="1">
+        <v>42987</v>
+      </c>
+      <c r="F548" s="2">
+        <v>2364</v>
+      </c>
+      <c r="G548" s="3">
+        <v>150000</v>
       </c>
       <c r="H548" s="3">
         <f t="shared" si="41"/>
-        <v>-150000</v>
+        <v>0</v>
       </c>
       <c r="I548" s="4">
         <f t="shared" si="43"/>
-        <v>1900</v>
+        <v>2017</v>
       </c>
       <c r="J548">
         <f t="shared" si="44"/>
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="549" spans="1:10">
@@ -35986,20 +37132,35 @@
         <f t="shared" si="42"/>
         <v>548</v>
       </c>
+      <c r="B549" t="s">
+        <v>106</v>
+      </c>
       <c r="C549">
         <v>1</v>
+      </c>
+      <c r="D549">
+        <v>10</v>
+      </c>
+      <c r="E549" s="1">
+        <v>43022</v>
+      </c>
+      <c r="F549" s="2">
+        <v>2538</v>
+      </c>
+      <c r="G549" s="3">
+        <v>150000</v>
       </c>
       <c r="H549" s="3">
         <f t="shared" si="41"/>
-        <v>-150000</v>
+        <v>0</v>
       </c>
       <c r="I549" s="4">
         <f t="shared" si="43"/>
-        <v>1900</v>
+        <v>2017</v>
       </c>
       <c r="J549">
         <f t="shared" si="44"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="550" spans="1:10">
@@ -36007,20 +37168,35 @@
         <f t="shared" si="42"/>
         <v>549</v>
       </c>
+      <c r="B550" t="s">
+        <v>106</v>
+      </c>
       <c r="C550">
         <v>1</v>
+      </c>
+      <c r="D550">
+        <v>11</v>
+      </c>
+      <c r="E550" s="1">
+        <v>43071</v>
+      </c>
+      <c r="F550" s="2">
+        <v>2618</v>
+      </c>
+      <c r="G550" s="3">
+        <v>150000</v>
       </c>
       <c r="H550" s="3">
         <f t="shared" si="41"/>
-        <v>-150000</v>
+        <v>0</v>
       </c>
       <c r="I550" s="4">
         <f t="shared" si="43"/>
-        <v>1900</v>
+        <v>2017</v>
       </c>
       <c r="J550">
         <f t="shared" si="44"/>
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="551" spans="1:10">
@@ -36028,16 +37204,31 @@
         <f t="shared" si="42"/>
         <v>550</v>
       </c>
+      <c r="B551" t="s">
+        <v>106</v>
+      </c>
       <c r="C551">
         <v>1</v>
+      </c>
+      <c r="D551">
+        <v>12</v>
+      </c>
+      <c r="E551" s="1">
+        <v>43104</v>
+      </c>
+      <c r="F551" s="2">
+        <v>2713</v>
+      </c>
+      <c r="G551" s="3">
+        <v>150000</v>
       </c>
       <c r="H551" s="3">
         <f t="shared" si="41"/>
-        <v>-150000</v>
+        <v>0</v>
       </c>
       <c r="I551" s="4">
         <f t="shared" si="43"/>
-        <v>1900</v>
+        <v>2018</v>
       </c>
       <c r="J551">
         <f t="shared" si="44"/>
@@ -36049,20 +37240,35 @@
         <f t="shared" si="42"/>
         <v>551</v>
       </c>
+      <c r="B552" t="s">
+        <v>107</v>
+      </c>
       <c r="C552">
         <v>1</v>
+      </c>
+      <c r="D552">
+        <v>7</v>
+      </c>
+      <c r="E552" s="1">
+        <v>42938</v>
+      </c>
+      <c r="F552" s="2">
+        <v>1232</v>
+      </c>
+      <c r="G552" s="3">
+        <v>150000</v>
       </c>
       <c r="H552" s="3">
         <f t="shared" si="41"/>
-        <v>-150000</v>
+        <v>0</v>
       </c>
       <c r="I552" s="4">
         <f t="shared" si="43"/>
-        <v>1900</v>
+        <v>2017</v>
       </c>
       <c r="J552">
         <f t="shared" si="44"/>
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="553" spans="1:10">
@@ -36070,20 +37276,35 @@
         <f t="shared" si="42"/>
         <v>552</v>
       </c>
+      <c r="B553" t="s">
+        <v>107</v>
+      </c>
       <c r="C553">
         <v>1</v>
+      </c>
+      <c r="D553">
+        <v>8</v>
+      </c>
+      <c r="E553" s="1">
+        <v>42959</v>
+      </c>
+      <c r="F553" s="2">
+        <v>2283</v>
+      </c>
+      <c r="G553" s="3">
+        <v>150000</v>
       </c>
       <c r="H553" s="3">
         <f t="shared" si="41"/>
-        <v>-150000</v>
+        <v>0</v>
       </c>
       <c r="I553" s="4">
         <f t="shared" si="43"/>
-        <v>1900</v>
+        <v>2017</v>
       </c>
       <c r="J553">
         <f t="shared" si="44"/>
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="554" spans="1:10">
@@ -36091,20 +37312,35 @@
         <f t="shared" si="42"/>
         <v>553</v>
       </c>
+      <c r="B554" t="s">
+        <v>107</v>
+      </c>
       <c r="C554">
         <v>1</v>
+      </c>
+      <c r="D554">
+        <v>9</v>
+      </c>
+      <c r="E554" s="1">
+        <v>42987</v>
+      </c>
+      <c r="F554" s="2">
+        <v>2380</v>
+      </c>
+      <c r="G554" s="3">
+        <v>150000</v>
       </c>
       <c r="H554" s="3">
         <f t="shared" si="41"/>
-        <v>-150000</v>
+        <v>0</v>
       </c>
       <c r="I554" s="4">
         <f t="shared" si="43"/>
-        <v>1900</v>
+        <v>2017</v>
       </c>
       <c r="J554">
         <f t="shared" si="44"/>
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="555" spans="1:10">
@@ -36112,20 +37348,35 @@
         <f t="shared" si="42"/>
         <v>554</v>
       </c>
+      <c r="B555" t="s">
+        <v>107</v>
+      </c>
       <c r="C555">
         <v>1</v>
+      </c>
+      <c r="D555">
+        <v>10</v>
+      </c>
+      <c r="E555" s="1">
+        <v>43014</v>
+      </c>
+      <c r="F555" s="2">
+        <v>2448</v>
+      </c>
+      <c r="G555" s="3">
+        <v>150000</v>
       </c>
       <c r="H555" s="3">
         <f t="shared" si="41"/>
-        <v>-150000</v>
+        <v>0</v>
       </c>
       <c r="I555" s="4">
         <f t="shared" si="43"/>
-        <v>1900</v>
+        <v>2017</v>
       </c>
       <c r="J555">
         <f t="shared" si="44"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="556" spans="1:10">
@@ -36133,20 +37384,35 @@
         <f t="shared" si="42"/>
         <v>555</v>
       </c>
+      <c r="B556" t="s">
+        <v>107</v>
+      </c>
       <c r="C556">
         <v>1</v>
+      </c>
+      <c r="D556">
+        <v>11</v>
+      </c>
+      <c r="E556" s="1">
+        <v>43050</v>
+      </c>
+      <c r="F556" s="2">
+        <v>2497</v>
+      </c>
+      <c r="G556" s="3">
+        <v>150000</v>
       </c>
       <c r="H556" s="3">
         <f t="shared" si="41"/>
-        <v>-150000</v>
+        <v>0</v>
       </c>
       <c r="I556" s="4">
         <f t="shared" si="43"/>
-        <v>1900</v>
+        <v>2017</v>
       </c>
       <c r="J556">
         <f t="shared" si="44"/>
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="557" spans="1:10">
@@ -36154,20 +37420,35 @@
         <f t="shared" si="42"/>
         <v>556</v>
       </c>
+      <c r="B557" t="s">
+        <v>107</v>
+      </c>
       <c r="C557">
         <v>1</v>
+      </c>
+      <c r="D557">
+        <v>12</v>
+      </c>
+      <c r="E557" s="1">
+        <v>43078</v>
+      </c>
+      <c r="F557" s="2">
+        <v>2621</v>
+      </c>
+      <c r="G557" s="3">
+        <v>150000</v>
       </c>
       <c r="H557" s="3">
         <f t="shared" si="41"/>
-        <v>-150000</v>
+        <v>0</v>
       </c>
       <c r="I557" s="4">
         <f t="shared" si="43"/>
-        <v>1900</v>
+        <v>2017</v>
       </c>
       <c r="J557">
         <f t="shared" si="44"/>
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="558" spans="1:10">
@@ -36175,20 +37456,35 @@
         <f t="shared" si="42"/>
         <v>557</v>
       </c>
+      <c r="B558" t="s">
+        <v>107</v>
+      </c>
       <c r="C558">
         <v>1</v>
+      </c>
+      <c r="D558">
+        <v>1</v>
+      </c>
+      <c r="E558" s="1">
+        <v>43141</v>
+      </c>
+      <c r="F558" s="2">
+        <v>2789</v>
+      </c>
+      <c r="G558" s="3">
+        <v>150000</v>
       </c>
       <c r="H558" s="3">
         <f t="shared" si="41"/>
-        <v>-150000</v>
+        <v>0</v>
       </c>
       <c r="I558" s="4">
         <f t="shared" si="43"/>
-        <v>1900</v>
+        <v>2018</v>
       </c>
       <c r="J558">
         <f t="shared" si="44"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="559" spans="1:10">
@@ -36196,20 +37492,35 @@
         <f t="shared" si="42"/>
         <v>558</v>
       </c>
+      <c r="B559" t="s">
+        <v>107</v>
+      </c>
       <c r="C559">
         <v>1</v>
+      </c>
+      <c r="D559">
+        <v>2</v>
+      </c>
+      <c r="E559" s="1">
+        <v>43141</v>
+      </c>
+      <c r="F559" s="2">
+        <v>2789</v>
+      </c>
+      <c r="G559" s="3">
+        <v>150000</v>
       </c>
       <c r="H559" s="3">
         <f t="shared" si="41"/>
-        <v>-150000</v>
+        <v>0</v>
       </c>
       <c r="I559" s="4">
         <f t="shared" si="43"/>
-        <v>1900</v>
+        <v>2018</v>
       </c>
       <c r="J559">
         <f t="shared" si="44"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="560" spans="1:10">
@@ -36217,20 +37528,35 @@
         <f t="shared" si="42"/>
         <v>559</v>
       </c>
+      <c r="B560" t="s">
+        <v>108</v>
+      </c>
       <c r="C560">
         <v>1</v>
+      </c>
+      <c r="D560">
+        <v>9</v>
+      </c>
+      <c r="E560" s="1">
+        <v>42983</v>
+      </c>
+      <c r="F560" s="2">
+        <v>2269</v>
+      </c>
+      <c r="G560" s="3">
+        <v>150000</v>
       </c>
       <c r="H560" s="3">
         <f t="shared" si="41"/>
-        <v>-150000</v>
+        <v>0</v>
       </c>
       <c r="I560" s="4">
         <f t="shared" si="43"/>
-        <v>1900</v>
+        <v>2017</v>
       </c>
       <c r="J560">
         <f t="shared" si="44"/>
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="561" spans="1:10">
@@ -36238,20 +37564,35 @@
         <f t="shared" si="42"/>
         <v>560</v>
       </c>
+      <c r="B561" t="s">
+        <v>108</v>
+      </c>
       <c r="C561">
         <v>1</v>
+      </c>
+      <c r="D561">
+        <v>10</v>
+      </c>
+      <c r="E561" s="1">
+        <v>43022</v>
+      </c>
+      <c r="F561" s="2">
+        <v>2537</v>
+      </c>
+      <c r="G561" s="3">
+        <v>150000</v>
       </c>
       <c r="H561" s="3">
         <f t="shared" si="41"/>
-        <v>-150000</v>
+        <v>0</v>
       </c>
       <c r="I561" s="4">
         <f t="shared" si="43"/>
-        <v>1900</v>
+        <v>2017</v>
       </c>
       <c r="J561">
         <f t="shared" si="44"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="562" spans="1:10">
@@ -36259,20 +37600,35 @@
         <f t="shared" si="42"/>
         <v>561</v>
       </c>
+      <c r="B562" t="s">
+        <v>108</v>
+      </c>
       <c r="C562">
         <v>1</v>
+      </c>
+      <c r="D562">
+        <v>11</v>
+      </c>
+      <c r="E562" s="1">
+        <v>43043</v>
+      </c>
+      <c r="F562" s="2">
+        <v>2485</v>
+      </c>
+      <c r="G562" s="3">
+        <v>150000</v>
       </c>
       <c r="H562" s="3">
         <f t="shared" si="41"/>
-        <v>-150000</v>
+        <v>0</v>
       </c>
       <c r="I562" s="4">
         <f t="shared" si="43"/>
-        <v>1900</v>
+        <v>2017</v>
       </c>
       <c r="J562">
         <f t="shared" si="44"/>
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="563" spans="1:10">
@@ -36280,20 +37636,35 @@
         <f t="shared" si="42"/>
         <v>562</v>
       </c>
+      <c r="B563" t="s">
+        <v>108</v>
+      </c>
       <c r="C563">
         <v>1</v>
+      </c>
+      <c r="D563">
+        <v>12</v>
+      </c>
+      <c r="E563" s="1">
+        <v>43085</v>
+      </c>
+      <c r="F563" s="2">
+        <v>2641</v>
+      </c>
+      <c r="G563" s="3">
+        <v>150000</v>
       </c>
       <c r="H563" s="3">
         <f t="shared" si="41"/>
-        <v>-150000</v>
+        <v>0</v>
       </c>
       <c r="I563" s="4">
         <f t="shared" si="43"/>
-        <v>1900</v>
+        <v>2017</v>
       </c>
       <c r="J563">
         <f t="shared" si="44"/>
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="564" spans="1:10">
@@ -36301,20 +37672,35 @@
         <f t="shared" si="42"/>
         <v>563</v>
       </c>
+      <c r="B564" t="s">
+        <v>108</v>
+      </c>
       <c r="C564">
         <v>1</v>
+      </c>
+      <c r="D564">
+        <v>1</v>
+      </c>
+      <c r="E564" s="1">
+        <v>43134</v>
+      </c>
+      <c r="F564" s="2">
+        <v>2773</v>
+      </c>
+      <c r="G564" s="3">
+        <v>150000</v>
       </c>
       <c r="H564" s="3">
         <f t="shared" si="41"/>
-        <v>-150000</v>
+        <v>0</v>
       </c>
       <c r="I564" s="4">
         <f t="shared" si="43"/>
-        <v>1900</v>
+        <v>2018</v>
       </c>
       <c r="J564">
         <f t="shared" si="44"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="565" spans="1:10">
@@ -36322,20 +37708,35 @@
         <f t="shared" si="42"/>
         <v>564</v>
       </c>
+      <c r="B565" t="s">
+        <v>109</v>
+      </c>
       <c r="C565">
         <v>1</v>
+      </c>
+      <c r="D565">
+        <v>9</v>
+      </c>
+      <c r="E565" s="1">
+        <v>42952</v>
+      </c>
+      <c r="F565" s="2">
+        <v>2262</v>
+      </c>
+      <c r="G565" s="3">
+        <v>120000</v>
       </c>
       <c r="H565" s="3">
         <f t="shared" si="41"/>
-        <v>-150000</v>
+        <v>-30000</v>
       </c>
       <c r="I565" s="4">
         <f t="shared" si="43"/>
-        <v>1900</v>
+        <v>2017</v>
       </c>
       <c r="J565">
         <f t="shared" si="44"/>
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="566" spans="1:10">
@@ -36343,20 +37744,35 @@
         <f t="shared" si="42"/>
         <v>565</v>
       </c>
+      <c r="B566" t="s">
+        <v>109</v>
+      </c>
       <c r="C566">
         <v>1</v>
+      </c>
+      <c r="D566">
+        <v>10</v>
+      </c>
+      <c r="E566" s="1">
+        <v>43008</v>
+      </c>
+      <c r="F566" s="2">
+        <v>2391</v>
+      </c>
+      <c r="G566" s="3">
+        <v>120000</v>
       </c>
       <c r="H566" s="3">
         <f t="shared" si="41"/>
-        <v>-150000</v>
+        <v>-30000</v>
       </c>
       <c r="I566" s="4">
         <f t="shared" si="43"/>
-        <v>1900</v>
+        <v>2017</v>
       </c>
       <c r="J566">
         <f t="shared" si="44"/>
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="567" spans="1:10">
@@ -36364,20 +37780,35 @@
         <f t="shared" si="42"/>
         <v>566</v>
       </c>
+      <c r="B567" t="s">
+        <v>109</v>
+      </c>
       <c r="C567">
         <v>1</v>
+      </c>
+      <c r="D567">
+        <v>11</v>
+      </c>
+      <c r="E567" s="1">
+        <v>43064</v>
+      </c>
+      <c r="F567" s="2">
+        <v>2599</v>
+      </c>
+      <c r="G567" s="3">
+        <v>120000</v>
       </c>
       <c r="H567" s="3">
         <f t="shared" si="41"/>
-        <v>-150000</v>
+        <v>-30000</v>
       </c>
       <c r="I567" s="4">
         <f t="shared" si="43"/>
-        <v>1900</v>
+        <v>2017</v>
       </c>
       <c r="J567">
         <f t="shared" si="44"/>
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="568" spans="1:10">
@@ -36385,20 +37816,35 @@
         <f t="shared" si="42"/>
         <v>567</v>
       </c>
+      <c r="B568" t="s">
+        <v>109</v>
+      </c>
       <c r="C568">
         <v>1</v>
+      </c>
+      <c r="D568">
+        <v>12</v>
+      </c>
+      <c r="E568" s="1">
+        <v>43064</v>
+      </c>
+      <c r="F568" s="2">
+        <v>2599</v>
+      </c>
+      <c r="G568" s="3">
+        <v>120000</v>
       </c>
       <c r="H568" s="3">
         <f t="shared" si="41"/>
-        <v>-150000</v>
+        <v>-30000</v>
       </c>
       <c r="I568" s="4">
         <f t="shared" si="43"/>
-        <v>1900</v>
+        <v>2017</v>
       </c>
       <c r="J568">
         <f t="shared" si="44"/>
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="569" spans="1:10">
@@ -36406,20 +37852,35 @@
         <f t="shared" si="42"/>
         <v>568</v>
       </c>
+      <c r="B569" t="s">
+        <v>109</v>
+      </c>
       <c r="C569">
         <v>1</v>
+      </c>
+      <c r="D569">
+        <v>1</v>
+      </c>
+      <c r="E569" s="1">
+        <v>43141</v>
+      </c>
+      <c r="F569" s="2">
+        <v>2793</v>
+      </c>
+      <c r="G569" s="3">
+        <v>120000</v>
       </c>
       <c r="H569" s="3">
         <f t="shared" si="41"/>
-        <v>-150000</v>
+        <v>-30000</v>
       </c>
       <c r="I569" s="4">
         <f t="shared" si="43"/>
-        <v>1900</v>
+        <v>2018</v>
       </c>
       <c r="J569">
         <f t="shared" si="44"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="570" spans="1:10">
@@ -36427,20 +37888,35 @@
         <f t="shared" si="42"/>
         <v>569</v>
       </c>
+      <c r="B570" t="s">
+        <v>109</v>
+      </c>
       <c r="C570">
         <v>1</v>
+      </c>
+      <c r="D570">
+        <v>2</v>
+      </c>
+      <c r="E570" s="1">
+        <v>43141</v>
+      </c>
+      <c r="F570" s="2">
+        <v>2793</v>
+      </c>
+      <c r="G570" s="3">
+        <v>120000</v>
       </c>
       <c r="H570" s="3">
         <f t="shared" si="41"/>
-        <v>-150000</v>
+        <v>-30000</v>
       </c>
       <c r="I570" s="4">
         <f t="shared" si="43"/>
-        <v>1900</v>
+        <v>2018</v>
       </c>
       <c r="J570">
         <f t="shared" si="44"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="571" spans="1:10">

</xml_diff>